<commit_message>
Ingreso de las demás bd y aplicación
</commit_message>
<xml_diff>
--- a/dat/ALGORITMOS_CLINICOS_NEW_ZC.xlsx
+++ b/dat/ALGORITMOS_CLINICOS_NEW_ZC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zulmacucunuba/Documents/GIT/quality-rips-surveillance/dat/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e5f934af0bcd737c/Documentos/DanielaBM/2023/3. Trabajo/Asistente investigativo PUJ/quality-rips-surveillance/quality-rips-surveillance/dat/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B01C450D-70C7-0044-9E33-D5993F264880}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="165" documentId="8_{B01C450D-70C7-0044-9E33-D5993F264880}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C4126A52-57B1-4E14-8A7F-F5E216533D4C}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="1440" windowWidth="27240" windowHeight="14760" xr2:uid="{397AFB3D-8797-9649-AC57-B2DA0DFEFF5D}"/>
+    <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="10170" xr2:uid="{397AFB3D-8797-9649-AC57-B2DA0DFEFF5D}"/>
   </bookViews>
   <sheets>
     <sheet name="DM" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="270">
   <si>
     <t>CODIGO_SIGNIFICADO</t>
   </si>
@@ -415,9 +415,6 @@
     <t>M142</t>
   </si>
   <si>
-    <t xml:space="preserve"> DE ACCIÓN PROLONGADA</t>
-  </si>
-  <si>
     <t>A10AE01</t>
   </si>
   <si>
@@ -742,31 +739,115 @@
     <t>A10BD03</t>
   </si>
   <si>
-    <t>NITORIZACION CONTINUA DE GLUCOSA</t>
-  </si>
-  <si>
     <t>GLUCOMETRIA</t>
   </si>
   <si>
-    <t>TIRAS REACTIVAS DE GLUCOMETRIA</t>
-  </si>
-  <si>
-    <t>LANCETAS</t>
-  </si>
-  <si>
-    <t>BOMBA DE INSULINA</t>
-  </si>
-  <si>
     <t>CODIGO</t>
   </si>
   <si>
     <t>ROOT</t>
   </si>
   <si>
+    <t>ATC</t>
+  </si>
+  <si>
+    <t>INSULINA Y ANALOGOS DE ACCIÓN PROLONGADA</t>
+  </si>
+  <si>
+    <t>MONITORIZACION CONTINUA DE GLUCOSA</t>
+  </si>
+  <si>
+    <t>INSULINA PRE Y POST GLUCOSA</t>
+  </si>
+  <si>
+    <t>INSULINA CURVA (CINCO MUESTRAS)</t>
+  </si>
+  <si>
+    <t>HEMOGLOBINA GLICOSILADA AUTOMATIZADA</t>
+  </si>
+  <si>
+    <t>HEMOGLOBINA GLICOSILADA MANUAL O SEMIAUTOMATIZADA</t>
+  </si>
+  <si>
+    <t>diab</t>
+  </si>
+  <si>
     <t>insul</t>
   </si>
   <si>
-    <t>sitaglip</t>
+    <t>sitag</t>
+  </si>
+  <si>
+    <t>vildag</t>
+  </si>
+  <si>
+    <t>saxag</t>
+  </si>
+  <si>
+    <t>linagl</t>
+  </si>
+  <si>
+    <t>alogl</t>
+  </si>
+  <si>
+    <t>gemiglip</t>
+  </si>
+  <si>
+    <t>canaglif</t>
+  </si>
+  <si>
+    <t>empaglif</t>
+  </si>
+  <si>
+    <t>dapaglif</t>
+  </si>
+  <si>
+    <t>metfor</t>
+  </si>
+  <si>
+    <t>fenfor</t>
+  </si>
+  <si>
+    <t>rosigli</t>
+  </si>
+  <si>
+    <t>pioglita</t>
+  </si>
+  <si>
+    <t>troglita</t>
+  </si>
+  <si>
+    <t>acarbo</t>
+  </si>
+  <si>
+    <t>miglit</t>
+  </si>
+  <si>
+    <t>clorpro</t>
+  </si>
+  <si>
+    <t>tolbut</t>
+  </si>
+  <si>
+    <t>glibencla</t>
+  </si>
+  <si>
+    <t>glimepi</t>
+  </si>
+  <si>
+    <t>gliclaz</t>
+  </si>
+  <si>
+    <t>glipiz</t>
+  </si>
+  <si>
+    <t>antidiabetico</t>
+  </si>
+  <si>
+    <t>gluco</t>
+  </si>
+  <si>
+    <t>hemog</t>
   </si>
 </sst>
 </file>
@@ -821,8 +902,12 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1118,32 +1203,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3478553-F71F-AA43-AE48-761FD61CF1E4}">
-  <dimension ref="A1:D128"/>
+  <dimension ref="A1:D129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
-      <selection activeCell="D89" sqref="D89:D125"/>
+    <sheetView tabSelected="1" topLeftCell="A113" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="E129" sqref="E129"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="76.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1153,8 +1238,11 @@
       <c r="C2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D2" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1164,8 +1252,11 @@
       <c r="C3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D3" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1175,8 +1266,11 @@
       <c r="C4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D4" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1186,8 +1280,11 @@
       <c r="C5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D5" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1197,8 +1294,11 @@
       <c r="C6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D6" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1208,8 +1308,11 @@
       <c r="C7" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D7" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -1219,8 +1322,11 @@
       <c r="C8" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D8" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -1230,8 +1336,11 @@
       <c r="C9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D9" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -1241,8 +1350,11 @@
       <c r="C10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D10" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -1252,8 +1364,11 @@
       <c r="C11" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D11" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -1263,8 +1378,11 @@
       <c r="C12" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D12" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -1274,8 +1392,11 @@
       <c r="C13" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D13" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -1285,8 +1406,11 @@
       <c r="C14" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D14" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -1296,8 +1420,11 @@
       <c r="C15" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D15" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>31</v>
       </c>
@@ -1307,8 +1434,11 @@
       <c r="C16" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>33</v>
       </c>
@@ -1318,8 +1448,11 @@
       <c r="C17" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D17" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -1329,8 +1462,11 @@
       <c r="C18" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D18" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>37</v>
       </c>
@@ -1340,8 +1476,11 @@
       <c r="C19" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D19" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>39</v>
       </c>
@@ -1351,8 +1490,11 @@
       <c r="C20" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D20" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>41</v>
       </c>
@@ -1362,8 +1504,11 @@
       <c r="C21" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D21" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>43</v>
       </c>
@@ -1373,8 +1518,11 @@
       <c r="C22" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D22" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>45</v>
       </c>
@@ -1384,8 +1532,11 @@
       <c r="C23" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D23" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>47</v>
       </c>
@@ -1395,8 +1546,11 @@
       <c r="C24" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D24" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>49</v>
       </c>
@@ -1406,8 +1560,11 @@
       <c r="C25" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D25" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>51</v>
       </c>
@@ -1417,8 +1574,11 @@
       <c r="C26" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D26" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>53</v>
       </c>
@@ -1428,8 +1588,11 @@
       <c r="C27" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D27" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>55</v>
       </c>
@@ -1439,8 +1602,11 @@
       <c r="C28" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D28" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>57</v>
       </c>
@@ -1450,8 +1616,11 @@
       <c r="C29" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D29" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>59</v>
       </c>
@@ -1461,8 +1630,11 @@
       <c r="C30" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D30" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>61</v>
       </c>
@@ -1472,8 +1644,11 @@
       <c r="C31" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D31" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>63</v>
       </c>
@@ -1483,8 +1658,11 @@
       <c r="C32" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D32" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>65</v>
       </c>
@@ -1494,8 +1672,11 @@
       <c r="C33" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D33" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>67</v>
       </c>
@@ -1505,8 +1686,11 @@
       <c r="C34" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D34" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>69</v>
       </c>
@@ -1516,8 +1700,11 @@
       <c r="C35" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D35" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>71</v>
       </c>
@@ -1527,8 +1714,11 @@
       <c r="C36" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D36" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>73</v>
       </c>
@@ -1538,8 +1728,11 @@
       <c r="C37" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D37" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>75</v>
       </c>
@@ -1549,8 +1742,11 @@
       <c r="C38" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D38" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>77</v>
       </c>
@@ -1560,8 +1756,11 @@
       <c r="C39" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D39" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>79</v>
       </c>
@@ -1571,8 +1770,11 @@
       <c r="C40" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D40" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>81</v>
       </c>
@@ -1582,8 +1784,11 @@
       <c r="C41" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D41" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>83</v>
       </c>
@@ -1593,8 +1798,11 @@
       <c r="C42" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D42" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>85</v>
       </c>
@@ -1604,8 +1812,11 @@
       <c r="C43" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D43" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>87</v>
       </c>
@@ -1615,8 +1826,11 @@
       <c r="C44" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D44" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>89</v>
       </c>
@@ -1626,8 +1840,11 @@
       <c r="C45" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D45" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>91</v>
       </c>
@@ -1637,8 +1854,11 @@
       <c r="C46" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D46" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>93</v>
       </c>
@@ -1648,8 +1868,11 @@
       <c r="C47" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D47" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>95</v>
       </c>
@@ -1659,8 +1882,11 @@
       <c r="C48" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D48" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>97</v>
       </c>
@@ -1670,8 +1896,11 @@
       <c r="C49" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D49" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>99</v>
       </c>
@@ -1681,8 +1910,11 @@
       <c r="C50" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D50" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>101</v>
       </c>
@@ -1692,8 +1924,11 @@
       <c r="C51" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D51" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>103</v>
       </c>
@@ -1703,8 +1938,11 @@
       <c r="C52" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D52" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>105</v>
       </c>
@@ -1714,8 +1952,11 @@
       <c r="C53" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D53" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>107</v>
       </c>
@@ -1725,8 +1966,11 @@
       <c r="C54" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D54" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>109</v>
       </c>
@@ -1736,8 +1980,11 @@
       <c r="C55" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D55" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>111</v>
       </c>
@@ -1747,8 +1994,11 @@
       <c r="C56" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D56" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>113</v>
       </c>
@@ -1758,8 +2008,11 @@
       <c r="C57" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D57" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>115</v>
       </c>
@@ -1769,8 +2022,11 @@
       <c r="C58" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D58" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>117</v>
       </c>
@@ -1780,8 +2036,11 @@
       <c r="C59" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D59" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>119</v>
       </c>
@@ -1791,8 +2050,11 @@
       <c r="C60" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D60" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>121</v>
       </c>
@@ -1802,8 +2064,11 @@
       <c r="C61" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D61" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>123</v>
       </c>
@@ -1813,896 +2078,946 @@
       <c r="C62" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D62" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
+        <v>237</v>
+      </c>
+      <c r="B63" t="s">
         <v>125</v>
       </c>
-      <c r="B63" t="s">
-        <v>126</v>
-      </c>
       <c r="C63" t="s">
+        <v>236</v>
+      </c>
+      <c r="D63" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
         <v>127</v>
       </c>
-      <c r="D63" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
+      <c r="B64" t="s">
         <v>128</v>
       </c>
-      <c r="B64" t="s">
+      <c r="C64" t="s">
+        <v>236</v>
+      </c>
+      <c r="D64" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
         <v>129</v>
       </c>
-      <c r="C64" t="s">
-        <v>127</v>
-      </c>
-      <c r="D64" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
+      <c r="B65" t="s">
         <v>130</v>
       </c>
-      <c r="B65" t="s">
+      <c r="C65" t="s">
+        <v>236</v>
+      </c>
+      <c r="D65" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>129</v>
+      </c>
+      <c r="B66" t="s">
         <v>131</v>
       </c>
-      <c r="C65" t="s">
-        <v>127</v>
-      </c>
-      <c r="D65" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
-        <v>130</v>
-      </c>
-      <c r="B66" t="s">
+      <c r="C66" t="s">
+        <v>236</v>
+      </c>
+      <c r="D66" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
         <v>132</v>
       </c>
-      <c r="C66" t="s">
-        <v>127</v>
-      </c>
-      <c r="D66" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
+      <c r="B67" t="s">
         <v>133</v>
       </c>
-      <c r="B67" t="s">
+      <c r="C67" t="s">
+        <v>236</v>
+      </c>
+      <c r="D67" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
         <v>134</v>
       </c>
-      <c r="C67" t="s">
-        <v>127</v>
-      </c>
-      <c r="D67" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
+      <c r="B68" t="s">
         <v>135</v>
       </c>
-      <c r="B68" t="s">
+      <c r="C68" t="s">
+        <v>236</v>
+      </c>
+      <c r="D68" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
         <v>136</v>
       </c>
-      <c r="C68" t="s">
-        <v>127</v>
-      </c>
-      <c r="D68" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
+      <c r="B69" t="s">
         <v>137</v>
       </c>
-      <c r="B69" t="s">
+      <c r="C69" t="s">
+        <v>236</v>
+      </c>
+      <c r="D69" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
         <v>138</v>
       </c>
-      <c r="C69" t="s">
-        <v>127</v>
-      </c>
-      <c r="D69" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
+      <c r="B70" t="s">
         <v>139</v>
       </c>
-      <c r="B70" t="s">
+      <c r="C70" t="s">
+        <v>236</v>
+      </c>
+      <c r="D70" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
         <v>140</v>
       </c>
-      <c r="C70" t="s">
-        <v>127</v>
-      </c>
-      <c r="D70" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
+      <c r="B71" t="s">
         <v>141</v>
       </c>
-      <c r="B71" t="s">
+      <c r="C71" t="s">
+        <v>236</v>
+      </c>
+      <c r="D71" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
         <v>142</v>
       </c>
-      <c r="C71" t="s">
-        <v>127</v>
-      </c>
-      <c r="D71" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
+      <c r="B72" t="s">
         <v>143</v>
       </c>
-      <c r="B72" t="s">
+      <c r="C72" t="s">
+        <v>236</v>
+      </c>
+      <c r="D72" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
+        <v>142</v>
+      </c>
+      <c r="B73" t="s">
         <v>144</v>
       </c>
-      <c r="C72" t="s">
-        <v>127</v>
-      </c>
-      <c r="D72" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
-        <v>143</v>
-      </c>
-      <c r="B73" t="s">
+      <c r="C73" t="s">
+        <v>236</v>
+      </c>
+      <c r="D73" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
+        <v>142</v>
+      </c>
+      <c r="B74" t="s">
         <v>145</v>
       </c>
-      <c r="C73" t="s">
-        <v>127</v>
-      </c>
-      <c r="D73" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
-        <v>143</v>
-      </c>
-      <c r="B74" t="s">
+      <c r="C74" t="s">
+        <v>236</v>
+      </c>
+      <c r="D74" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
+        <v>142</v>
+      </c>
+      <c r="B75" t="s">
         <v>146</v>
       </c>
-      <c r="C74" t="s">
-        <v>127</v>
-      </c>
-      <c r="D74" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A75" t="s">
-        <v>143</v>
-      </c>
-      <c r="B75" t="s">
+      <c r="C75" t="s">
+        <v>236</v>
+      </c>
+      <c r="D75" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
+        <v>142</v>
+      </c>
+      <c r="B76" t="s">
         <v>147</v>
       </c>
-      <c r="C75" t="s">
-        <v>127</v>
-      </c>
-      <c r="D75" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
-        <v>143</v>
-      </c>
-      <c r="B76" t="s">
+      <c r="C76" t="s">
+        <v>236</v>
+      </c>
+      <c r="D76" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
         <v>148</v>
       </c>
-      <c r="C76" t="s">
-        <v>127</v>
-      </c>
-      <c r="D76" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A77" t="s">
+      <c r="B77" t="s">
         <v>149</v>
       </c>
-      <c r="B77" t="s">
+      <c r="C77" t="s">
+        <v>236</v>
+      </c>
+      <c r="D77" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
+        <v>148</v>
+      </c>
+      <c r="B78" t="s">
         <v>150</v>
       </c>
-      <c r="C77" t="s">
-        <v>127</v>
-      </c>
-      <c r="D77" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A78" t="s">
-        <v>149</v>
-      </c>
-      <c r="B78" t="s">
+      <c r="C78" t="s">
+        <v>236</v>
+      </c>
+      <c r="D78" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
+        <v>148</v>
+      </c>
+      <c r="B79" t="s">
         <v>151</v>
       </c>
-      <c r="C78" t="s">
-        <v>127</v>
-      </c>
-      <c r="D78" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A79" t="s">
-        <v>149</v>
-      </c>
-      <c r="B79" t="s">
+      <c r="C79" t="s">
+        <v>236</v>
+      </c>
+      <c r="D79" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
+        <v>148</v>
+      </c>
+      <c r="B80" t="s">
         <v>152</v>
       </c>
-      <c r="C79" t="s">
-        <v>127</v>
-      </c>
-      <c r="D79" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A80" t="s">
-        <v>149</v>
-      </c>
-      <c r="B80" t="s">
+      <c r="C80" t="s">
+        <v>236</v>
+      </c>
+      <c r="D80" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
+        <v>148</v>
+      </c>
+      <c r="B81" t="s">
         <v>153</v>
       </c>
-      <c r="C80" t="s">
-        <v>127</v>
-      </c>
-      <c r="D80" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A81" t="s">
-        <v>149</v>
-      </c>
-      <c r="B81" t="s">
+      <c r="C81" t="s">
+        <v>236</v>
+      </c>
+      <c r="D81" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
+        <v>148</v>
+      </c>
+      <c r="B82" t="s">
         <v>154</v>
       </c>
-      <c r="C81" t="s">
-        <v>127</v>
-      </c>
-      <c r="D81" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A82" t="s">
-        <v>149</v>
-      </c>
-      <c r="B82" t="s">
+      <c r="C82" t="s">
+        <v>236</v>
+      </c>
+      <c r="D82" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
         <v>155</v>
       </c>
-      <c r="C82" t="s">
-        <v>127</v>
-      </c>
-      <c r="D82" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A83" t="s">
+      <c r="B83" t="s">
         <v>156</v>
       </c>
-      <c r="B83" t="s">
+      <c r="C83" t="s">
+        <v>236</v>
+      </c>
+      <c r="D83" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
+        <v>155</v>
+      </c>
+      <c r="B84" t="s">
         <v>157</v>
       </c>
-      <c r="C83" t="s">
-        <v>127</v>
-      </c>
-      <c r="D83" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A84" t="s">
-        <v>156</v>
-      </c>
-      <c r="B84" t="s">
+      <c r="C84" t="s">
+        <v>236</v>
+      </c>
+      <c r="D84" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
+        <v>155</v>
+      </c>
+      <c r="B85" t="s">
         <v>158</v>
       </c>
-      <c r="C84" t="s">
-        <v>127</v>
-      </c>
-      <c r="D84" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A85" t="s">
-        <v>156</v>
-      </c>
-      <c r="B85" t="s">
+      <c r="C85" t="s">
+        <v>236</v>
+      </c>
+      <c r="D85" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
         <v>159</v>
       </c>
-      <c r="C85" t="s">
-        <v>127</v>
-      </c>
-      <c r="D85" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A86" t="s">
+      <c r="B86" t="s">
         <v>160</v>
       </c>
-      <c r="B86" t="s">
+      <c r="C86" t="s">
+        <v>236</v>
+      </c>
+      <c r="D86" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
         <v>161</v>
       </c>
-      <c r="C86" t="s">
-        <v>127</v>
-      </c>
-      <c r="D86" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A87" t="s">
+      <c r="B87" t="s">
         <v>162</v>
       </c>
-      <c r="B87" t="s">
+      <c r="C87" t="s">
+        <v>236</v>
+      </c>
+      <c r="D87" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
         <v>163</v>
       </c>
-      <c r="C87" t="s">
-        <v>127</v>
-      </c>
-      <c r="D87" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A88" t="s">
+      <c r="B88" t="s">
         <v>164</v>
       </c>
-      <c r="B88" t="s">
+      <c r="C88" t="s">
+        <v>236</v>
+      </c>
+      <c r="D88" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
         <v>165</v>
       </c>
-      <c r="C88" t="s">
-        <v>127</v>
-      </c>
-      <c r="D88" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A89" t="s">
+      <c r="B89" t="s">
         <v>166</v>
       </c>
-      <c r="B89" t="s">
+      <c r="C89" t="s">
+        <v>236</v>
+      </c>
+      <c r="D89" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
         <v>167</v>
       </c>
-      <c r="C89" t="s">
-        <v>127</v>
-      </c>
-      <c r="D89" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A90" t="s">
+      <c r="B90" t="s">
         <v>168</v>
       </c>
-      <c r="B90" t="s">
+      <c r="C90" t="s">
+        <v>236</v>
+      </c>
+      <c r="D90" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
         <v>169</v>
       </c>
-      <c r="C90" t="s">
-        <v>127</v>
-      </c>
-      <c r="D90" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A91" t="s">
+      <c r="B91" t="s">
         <v>170</v>
       </c>
-      <c r="B91" t="s">
+      <c r="C91" t="s">
+        <v>236</v>
+      </c>
+      <c r="D91" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
         <v>171</v>
       </c>
-      <c r="C91" t="s">
-        <v>127</v>
-      </c>
-      <c r="D91" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A92" t="s">
+      <c r="B92" t="s">
         <v>172</v>
       </c>
-      <c r="B92" t="s">
+      <c r="C92" t="s">
+        <v>236</v>
+      </c>
+      <c r="D92" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A93" t="s">
         <v>173</v>
       </c>
-      <c r="C92" t="s">
-        <v>127</v>
-      </c>
-      <c r="D92" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A93" t="s">
+      <c r="B93" t="s">
         <v>174</v>
       </c>
-      <c r="B93" t="s">
+      <c r="C93" t="s">
+        <v>236</v>
+      </c>
+      <c r="D93" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
         <v>175</v>
       </c>
-      <c r="C93" t="s">
-        <v>127</v>
-      </c>
-      <c r="D93" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A94" t="s">
+      <c r="B94" t="s">
         <v>176</v>
       </c>
-      <c r="B94" t="s">
+      <c r="C94" t="s">
+        <v>236</v>
+      </c>
+      <c r="D94" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
         <v>177</v>
       </c>
-      <c r="C94" t="s">
-        <v>127</v>
-      </c>
-      <c r="D94" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A95" t="s">
+      <c r="B95" t="s">
         <v>178</v>
       </c>
-      <c r="B95" t="s">
+      <c r="C95" t="s">
+        <v>236</v>
+      </c>
+      <c r="D95" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
         <v>179</v>
       </c>
-      <c r="C95" t="s">
-        <v>127</v>
-      </c>
-      <c r="D95" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A96" t="s">
+      <c r="B96" t="s">
         <v>180</v>
       </c>
-      <c r="B96" t="s">
+      <c r="C96" t="s">
+        <v>236</v>
+      </c>
+      <c r="D96" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A97" t="s">
         <v>181</v>
       </c>
-      <c r="C96" t="s">
-        <v>127</v>
-      </c>
-      <c r="D96" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A97" t="s">
+      <c r="B97" t="s">
         <v>182</v>
       </c>
-      <c r="B97" t="s">
+      <c r="C97" t="s">
+        <v>236</v>
+      </c>
+      <c r="D97" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A98" t="s">
         <v>183</v>
       </c>
-      <c r="C97" t="s">
-        <v>127</v>
-      </c>
-      <c r="D97" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A98" t="s">
+      <c r="B98" t="s">
         <v>184</v>
       </c>
-      <c r="B98" t="s">
+      <c r="C98" t="s">
+        <v>236</v>
+      </c>
+      <c r="D98" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A99" t="s">
         <v>185</v>
       </c>
-      <c r="C98" t="s">
-        <v>127</v>
-      </c>
-      <c r="D98" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A99" t="s">
+      <c r="B99" t="s">
         <v>186</v>
       </c>
-      <c r="B99" t="s">
+      <c r="C99" t="s">
+        <v>236</v>
+      </c>
+      <c r="D99" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A100" t="s">
         <v>187</v>
       </c>
-      <c r="C99" t="s">
-        <v>127</v>
-      </c>
-      <c r="D99" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A100" t="s">
+      <c r="B100" t="s">
         <v>188</v>
       </c>
-      <c r="B100" t="s">
+      <c r="C100" t="s">
+        <v>236</v>
+      </c>
+      <c r="D100" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A101" t="s">
         <v>189</v>
       </c>
-      <c r="C100" t="s">
-        <v>127</v>
-      </c>
-      <c r="D100" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A101" t="s">
+      <c r="B101" t="s">
         <v>190</v>
       </c>
-      <c r="B101" t="s">
+      <c r="C101" t="s">
+        <v>236</v>
+      </c>
+      <c r="D101" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A102" t="s">
         <v>191</v>
       </c>
-      <c r="C101" t="s">
-        <v>127</v>
-      </c>
-      <c r="D101" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A102" t="s">
+      <c r="B102" t="s">
         <v>192</v>
       </c>
-      <c r="B102" t="s">
+      <c r="C102" t="s">
+        <v>236</v>
+      </c>
+      <c r="D102" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A103" t="s">
         <v>193</v>
       </c>
-      <c r="C102" t="s">
-        <v>127</v>
-      </c>
-      <c r="D102" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A103" t="s">
+      <c r="B103" t="s">
         <v>194</v>
       </c>
-      <c r="B103" t="s">
+      <c r="C103" t="s">
+        <v>236</v>
+      </c>
+      <c r="D103" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A104" t="s">
         <v>195</v>
       </c>
-      <c r="C103" t="s">
-        <v>127</v>
-      </c>
-      <c r="D103" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A104" t="s">
+      <c r="B104" t="s">
         <v>196</v>
       </c>
-      <c r="B104" t="s">
+      <c r="C104" t="s">
+        <v>236</v>
+      </c>
+      <c r="D104" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A105" t="s">
         <v>197</v>
       </c>
-      <c r="C104" t="s">
-        <v>127</v>
-      </c>
-      <c r="D104" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A105" t="s">
+      <c r="B105" t="s">
         <v>198</v>
       </c>
-      <c r="B105" t="s">
+      <c r="C105" t="s">
+        <v>236</v>
+      </c>
+      <c r="D105" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A106" t="s">
         <v>199</v>
       </c>
-      <c r="C105" t="s">
-        <v>127</v>
-      </c>
-      <c r="D105" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A106" t="s">
+      <c r="B106" t="s">
         <v>200</v>
       </c>
-      <c r="B106" t="s">
+      <c r="C106" t="s">
+        <v>236</v>
+      </c>
+      <c r="D106" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A107" t="s">
         <v>201</v>
       </c>
-      <c r="C106" t="s">
-        <v>127</v>
-      </c>
-      <c r="D106" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A107" t="s">
+      <c r="B107" t="s">
         <v>202</v>
       </c>
-      <c r="B107" t="s">
+      <c r="C107" t="s">
+        <v>236</v>
+      </c>
+      <c r="D107" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A108" t="s">
         <v>203</v>
       </c>
-      <c r="C107" t="s">
-        <v>127</v>
-      </c>
-      <c r="D107" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A108" t="s">
+      <c r="B108" t="s">
         <v>204</v>
       </c>
-      <c r="B108" t="s">
+      <c r="C108" t="s">
+        <v>236</v>
+      </c>
+      <c r="D108" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A109" t="s">
         <v>205</v>
       </c>
-      <c r="C108" t="s">
-        <v>127</v>
-      </c>
-      <c r="D108" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A109" t="s">
+      <c r="B109" t="s">
         <v>206</v>
       </c>
-      <c r="B109" t="s">
+      <c r="C109" t="s">
+        <v>236</v>
+      </c>
+      <c r="D109" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A110" t="s">
         <v>207</v>
       </c>
-      <c r="C109" t="s">
-        <v>127</v>
-      </c>
-      <c r="D109" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A110" t="s">
+      <c r="B110" t="s">
         <v>208</v>
       </c>
-      <c r="B110" t="s">
+      <c r="C110" t="s">
+        <v>236</v>
+      </c>
+      <c r="D110" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A111" t="s">
         <v>209</v>
       </c>
-      <c r="C110" t="s">
-        <v>127</v>
-      </c>
-      <c r="D110" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A111" t="s">
+      <c r="B111" t="s">
         <v>210</v>
       </c>
-      <c r="B111" t="s">
+      <c r="C111" t="s">
+        <v>236</v>
+      </c>
+      <c r="D111" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A112" t="s">
         <v>211</v>
       </c>
-      <c r="C111" t="s">
-        <v>127</v>
-      </c>
-      <c r="D111" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A112" t="s">
+      <c r="B112" t="s">
         <v>212</v>
       </c>
-      <c r="B112" t="s">
+      <c r="C112" t="s">
+        <v>236</v>
+      </c>
+      <c r="D112" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A113" t="s">
         <v>213</v>
       </c>
-      <c r="C112" t="s">
-        <v>127</v>
-      </c>
-      <c r="D112" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A113" t="s">
+      <c r="B113" t="s">
         <v>214</v>
       </c>
-      <c r="B113" t="s">
+      <c r="C113" t="s">
+        <v>236</v>
+      </c>
+      <c r="D113" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A114" t="s">
         <v>215</v>
       </c>
-      <c r="C113" t="s">
-        <v>127</v>
-      </c>
-      <c r="D113" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A114" t="s">
+      <c r="B114" t="s">
         <v>216</v>
       </c>
-      <c r="B114" t="s">
+      <c r="C114" t="s">
+        <v>236</v>
+      </c>
+      <c r="D114" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A115" t="s">
         <v>217</v>
       </c>
-      <c r="C114" t="s">
-        <v>127</v>
-      </c>
-      <c r="D114" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A115" t="s">
+      <c r="B115" t="s">
         <v>218</v>
       </c>
-      <c r="B115" t="s">
+      <c r="C115" t="s">
+        <v>236</v>
+      </c>
+      <c r="D115" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A116" t="s">
         <v>219</v>
       </c>
-      <c r="C115" t="s">
-        <v>127</v>
-      </c>
-      <c r="D115" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A116" t="s">
+      <c r="B116" t="s">
         <v>220</v>
       </c>
-      <c r="B116" t="s">
+      <c r="C116" t="s">
+        <v>236</v>
+      </c>
+      <c r="D116" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A117" t="s">
         <v>221</v>
       </c>
-      <c r="C116" t="s">
-        <v>127</v>
-      </c>
-      <c r="D116" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A117" t="s">
+      <c r="B117" t="s">
         <v>222</v>
       </c>
-      <c r="B117" t="s">
+      <c r="C117" t="s">
+        <v>236</v>
+      </c>
+      <c r="D117" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A118" t="s">
         <v>223</v>
       </c>
-      <c r="C117" t="s">
-        <v>127</v>
-      </c>
-      <c r="D117" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A118" t="s">
+      <c r="B118" t="s">
         <v>224</v>
       </c>
-      <c r="B118" t="s">
+      <c r="C118" t="s">
+        <v>236</v>
+      </c>
+      <c r="D118" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A119" t="s">
         <v>225</v>
       </c>
-      <c r="C118" t="s">
-        <v>127</v>
-      </c>
-      <c r="D118" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A119" t="s">
+      <c r="B119" t="s">
         <v>226</v>
       </c>
-      <c r="B119" t="s">
+      <c r="C119" t="s">
+        <v>236</v>
+      </c>
+      <c r="D119" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A120" t="s">
         <v>227</v>
       </c>
-      <c r="C119" t="s">
-        <v>127</v>
-      </c>
-      <c r="D119" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A120" t="s">
+      <c r="B120" t="s">
         <v>228</v>
       </c>
-      <c r="B120" t="s">
+      <c r="C120" t="s">
+        <v>236</v>
+      </c>
+      <c r="D120" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A121" t="s">
         <v>229</v>
       </c>
-      <c r="C120" t="s">
-        <v>127</v>
-      </c>
-      <c r="D120" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A121" t="s">
+      <c r="B121" t="s">
         <v>230</v>
       </c>
-      <c r="B121" t="s">
+      <c r="C121" t="s">
+        <v>236</v>
+      </c>
+      <c r="D121" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A122" t="s">
+        <v>229</v>
+      </c>
+      <c r="B122" t="s">
         <v>231</v>
       </c>
-      <c r="C121" t="s">
-        <v>127</v>
-      </c>
-      <c r="D121" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A122" t="s">
-        <v>230</v>
-      </c>
-      <c r="B122" t="s">
+      <c r="C122" t="s">
+        <v>236</v>
+      </c>
+      <c r="D122" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A123" t="s">
+        <v>229</v>
+      </c>
+      <c r="B123" t="s">
         <v>232</v>
       </c>
-      <c r="C122" t="s">
-        <v>127</v>
-      </c>
-      <c r="D122" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A123" t="s">
-        <v>230</v>
-      </c>
-      <c r="B123" t="s">
-        <v>233</v>
-      </c>
       <c r="C123" t="s">
-        <v>127</v>
+        <v>236</v>
       </c>
       <c r="D123" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="B124">
         <v>893911</v>
       </c>
+      <c r="C124" t="s">
+        <v>126</v>
+      </c>
       <c r="D124" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B125">
         <v>903883</v>
       </c>
+      <c r="C125" t="s">
+        <v>126</v>
+      </c>
       <c r="D125" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A126" t="s">
+        <v>239</v>
+      </c>
+      <c r="B126">
+        <v>904702</v>
+      </c>
+      <c r="C126" t="s">
+        <v>126</v>
+      </c>
+      <c r="D126" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A127" t="s">
+        <v>240</v>
+      </c>
+      <c r="B127">
+        <v>904703</v>
+      </c>
+      <c r="C127" t="s">
+        <v>126</v>
+      </c>
+      <c r="D127" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A128" t="s">
+        <v>241</v>
+      </c>
+      <c r="B128">
+        <v>903426</v>
+      </c>
+      <c r="C128" t="s">
+        <v>126</v>
+      </c>
+      <c r="D128" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A129" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A126" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A127" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A128" t="s">
-        <v>238</v>
+      <c r="B129">
+        <v>903427</v>
+      </c>
+      <c r="C129" t="s">
+        <v>126</v>
+      </c>
+      <c r="D129" t="s">
+        <v>269</v>
       </c>
     </row>
   </sheetData>
@@ -2714,9 +3029,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F7A4EE8-9C1A-4345-81FE-4CE18C64706F}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2730,7 +3045,7 @@
       <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Prev total, prev investigada.
</commit_message>
<xml_diff>
--- a/dat/ALGORITMOS_CLINICOS_NEW_ZC.xlsx
+++ b/dat/ALGORITMOS_CLINICOS_NEW_ZC.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e5f934af0bcd737c/Documentos/DanielaBM/2023/3. Trabajo/Asistente investigativo PUJ/quality-rips-surveillance/quality-rips-surveillance/dat/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="292" documentId="8_{B01C450D-70C7-0044-9E33-D5993F264880}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{364A19B9-CB90-4D19-9D91-0D5952B94F72}"/>
+  <xr:revisionPtr revIDLastSave="413" documentId="8_{B01C450D-70C7-0044-9E33-D5993F264880}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7AF148AD-E10A-4E45-A895-1CF070879DC9}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="9780" windowHeight="10170" activeTab="1" xr2:uid="{397AFB3D-8797-9649-AC57-B2DA0DFEFF5D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{397AFB3D-8797-9649-AC57-B2DA0DFEFF5D}"/>
   </bookViews>
   <sheets>
     <sheet name="DM" sheetId="1" r:id="rId1"/>
-    <sheet name="HTA" sheetId="2" r:id="rId2"/>
-    <sheet name="CANCER" sheetId="3" r:id="rId3"/>
+    <sheet name="ERC" sheetId="4" r:id="rId2"/>
+    <sheet name="HTA" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="898" uniqueCount="494">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1266" uniqueCount="636">
   <si>
     <t>CODIGO_SIGNIFICADO</t>
   </si>
@@ -1533,12 +1533,438 @@
   <si>
     <t>volol</t>
   </si>
+  <si>
+    <t>INSUFICIENCIA RENAL TERMINAL</t>
+  </si>
+  <si>
+    <t>N180</t>
+  </si>
+  <si>
+    <t>PARICALCITOL</t>
+  </si>
+  <si>
+    <t>A11CC07</t>
+  </si>
+  <si>
+    <t>CATETERIZACION VENOSA PARA DIALISIS RENAL SOD</t>
+  </si>
+  <si>
+    <t>OTRAS INSUFICIENCIAS RENALES CRONICAS</t>
+  </si>
+  <si>
+    <t>N188</t>
+  </si>
+  <si>
+    <t>SEVELAMER</t>
+  </si>
+  <si>
+    <t>V03AE02</t>
+  </si>
+  <si>
+    <t>FORMACION DE FISTULA AV (PERIFERICA) PARA DIALISIS RENAL</t>
+  </si>
+  <si>
+    <t>INSUFICIENCIA RENAL CRONICA, NO ESPECIFICADA</t>
+  </si>
+  <si>
+    <t>N189</t>
+  </si>
+  <si>
+    <t>FORMACION DE FISTULA AV (PERIFERICA) PARA DIALISIS RENAL CON PROTESIS[DERIVACION AV POR CANULA EXTERNA DE SCRIBNER] [INSERCION DE CANULA VASO A VASO]</t>
+  </si>
+  <si>
+    <t>INSUFICIENCIA RENAL NO ESPECIFICADA</t>
+  </si>
+  <si>
+    <t>N19</t>
+  </si>
+  <si>
+    <t>REVISION DE DERIVACION (FISTULA) ARTERIOVENOSA PARA DIALISIS RENAL SOD</t>
+  </si>
+  <si>
+    <t>ATORVASTATINA</t>
+  </si>
+  <si>
+    <t>C10AA05</t>
+  </si>
+  <si>
+    <t>EXTRACCION DE DERIVACION ARTERIOVENOSA PARA DIALISIS RENAL SOD</t>
+  </si>
+  <si>
+    <t>SIMVASTATINA</t>
+  </si>
+  <si>
+    <t>C10AA01</t>
+  </si>
+  <si>
+    <t>HEMODIALISIS ESTANDAR CON BICARBONATO</t>
+  </si>
+  <si>
+    <t>CERIVASTATINA</t>
+  </si>
+  <si>
+    <t>C10AA06</t>
+  </si>
+  <si>
+    <t>COLOCACION DE CATETER PARA DIALISIS PERITONEAL</t>
+  </si>
+  <si>
+    <t>PRAVASTATINA</t>
+  </si>
+  <si>
+    <t>C10AA03</t>
+  </si>
+  <si>
+    <t>INSERCION DE CATETER PERMANENTE PARA HEMODIALISIS</t>
+  </si>
+  <si>
+    <t>FLUVASTATINA</t>
+  </si>
+  <si>
+    <t>C10AA04</t>
+  </si>
+  <si>
+    <t>RETIRO DE CATETER PERMANENTE PARA HEMODIALISIS</t>
+  </si>
+  <si>
+    <t>ROSUVASTATINA</t>
+  </si>
+  <si>
+    <t>C10AA07</t>
+  </si>
+  <si>
+    <t>DIALISIS PERITONEAL SOD</t>
+  </si>
+  <si>
+    <t>LOVASTATINA</t>
+  </si>
+  <si>
+    <t>C10AA02</t>
+  </si>
+  <si>
+    <t>DIALISIS PERITONEAL MANUAL</t>
+  </si>
+  <si>
+    <t>CLOFIBRATO</t>
+  </si>
+  <si>
+    <t>C10AB01</t>
+  </si>
+  <si>
+    <t> EPROSARTÁN</t>
+  </si>
+  <si>
+    <t>DIALISIS PERITONEAL AUTOMATIZADA</t>
+  </si>
+  <si>
+    <t>BEZAFIBRATO</t>
+  </si>
+  <si>
+    <t>C10AB02</t>
+  </si>
+  <si>
+    <t> VALSARTÁN</t>
+  </si>
+  <si>
+    <t>SALA DE HEMODIALISIS</t>
+  </si>
+  <si>
+    <t>S22220</t>
+  </si>
+  <si>
+    <t>GEMFIBROZILO</t>
+  </si>
+  <si>
+    <t>C10AB04</t>
+  </si>
+  <si>
+    <t> IRBESARTÁN</t>
+  </si>
+  <si>
+    <t>SALA DE DIALISIS PERITONEAL</t>
+  </si>
+  <si>
+    <t>S22223</t>
+  </si>
+  <si>
+    <t>FENOFIBRATO</t>
+  </si>
+  <si>
+    <t>C10AB05</t>
+  </si>
+  <si>
+    <t>CIPROFIBRATO</t>
+  </si>
+  <si>
+    <t>C10AB08</t>
+  </si>
+  <si>
+    <t>COLECALCIFEROL</t>
+  </si>
+  <si>
+    <t>A11CC05</t>
+  </si>
+  <si>
+    <t>CALCITRIOL</t>
+  </si>
+  <si>
+    <t>A11CC04</t>
+  </si>
+  <si>
+    <t>CINACALCET</t>
+  </si>
+  <si>
+    <t>H05BX01</t>
+  </si>
+  <si>
+    <t>BICARBONATO DE SODIO</t>
+  </si>
+  <si>
+    <t>B05XA02</t>
+  </si>
+  <si>
+    <t>CARBONATO DE CALCIO</t>
+  </si>
+  <si>
+    <t>A02AC01</t>
+  </si>
+  <si>
+    <t>FUMARATO FERROSO</t>
+  </si>
+  <si>
+    <t>B03AA02</t>
+  </si>
+  <si>
+    <t>SULFATO FERROSO</t>
+  </si>
+  <si>
+    <t>B03AA07</t>
+  </si>
+  <si>
+    <t>ACIDO FOLICO</t>
+  </si>
+  <si>
+    <t>B03BB01</t>
+  </si>
+  <si>
+    <t>ERITROPOYETINA</t>
+  </si>
+  <si>
+    <t>B03XA01</t>
+  </si>
+  <si>
+    <t>EPOETINA BETA</t>
+  </si>
+  <si>
+    <t>B03XA03</t>
+  </si>
+  <si>
+    <t> FELODIPINO</t>
+  </si>
+  <si>
+    <t>POLIESTIRENO</t>
+  </si>
+  <si>
+    <t>V03AE01</t>
+  </si>
+  <si>
+    <t> ISRADIPINO</t>
+  </si>
+  <si>
+    <t> NICARDIPINO</t>
+  </si>
+  <si>
+    <t>NIFEDIPINO</t>
+  </si>
+  <si>
+    <t>C08CA05 </t>
+  </si>
+  <si>
+    <t> NIMODIPINO</t>
+  </si>
+  <si>
+    <t> NISOLDIPINO</t>
+  </si>
+  <si>
+    <t> NITRENDIPINO</t>
+  </si>
+  <si>
+    <t>insuficiencia</t>
+  </si>
+  <si>
+    <t>paracal</t>
+  </si>
+  <si>
+    <t>sevelam</t>
+  </si>
+  <si>
+    <t>lisinop</t>
+  </si>
+  <si>
+    <t>perendo</t>
+  </si>
+  <si>
+    <t>atorvas</t>
+  </si>
+  <si>
+    <t>simvast</t>
+  </si>
+  <si>
+    <t>cerivas</t>
+  </si>
+  <si>
+    <t>pravast</t>
+  </si>
+  <si>
+    <t>fluvast</t>
+  </si>
+  <si>
+    <t>rosuvas</t>
+  </si>
+  <si>
+    <t>lovasta</t>
+  </si>
+  <si>
+    <t>clofibr</t>
+  </si>
+  <si>
+    <t>bezafib</t>
+  </si>
+  <si>
+    <t>gemfibr</t>
+  </si>
+  <si>
+    <t>fenofib</t>
+  </si>
+  <si>
+    <t>ciprofi</t>
+  </si>
+  <si>
+    <t>colecal</t>
+  </si>
+  <si>
+    <t>calcitr</t>
+  </si>
+  <si>
+    <t>cinacal</t>
+  </si>
+  <si>
+    <t>bicarbo</t>
+  </si>
+  <si>
+    <t>carbona</t>
+  </si>
+  <si>
+    <t>fumarat</t>
+  </si>
+  <si>
+    <t>sulfato</t>
+  </si>
+  <si>
+    <t>acido f</t>
+  </si>
+  <si>
+    <t>eritrop</t>
+  </si>
+  <si>
+    <t>epoetin</t>
+  </si>
+  <si>
+    <t>poliest</t>
+  </si>
+  <si>
+    <t>captopr</t>
+  </si>
+  <si>
+    <t>enalapr</t>
+  </si>
+  <si>
+    <t>perindo</t>
+  </si>
+  <si>
+    <t>ramipri</t>
+  </si>
+  <si>
+    <t>quinapr</t>
+  </si>
+  <si>
+    <t>benazep</t>
+  </si>
+  <si>
+    <t>cilazap</t>
+  </si>
+  <si>
+    <t>fosinop</t>
+  </si>
+  <si>
+    <t>trandol</t>
+  </si>
+  <si>
+    <t>trandola</t>
+  </si>
+  <si>
+    <t>eprosar</t>
+  </si>
+  <si>
+    <t>valsart</t>
+  </si>
+  <si>
+    <t>irbesar</t>
+  </si>
+  <si>
+    <t>candesa</t>
+  </si>
+  <si>
+    <t>telmisa</t>
+  </si>
+  <si>
+    <t>olmesar</t>
+  </si>
+  <si>
+    <t>amlodip</t>
+  </si>
+  <si>
+    <t>felodip</t>
+  </si>
+  <si>
+    <t>isradip</t>
+  </si>
+  <si>
+    <t>nicardi</t>
+  </si>
+  <si>
+    <t>nifedip</t>
+  </si>
+  <si>
+    <t>nimodip</t>
+  </si>
+  <si>
+    <t>nisoldi</t>
+  </si>
+  <si>
+    <t>nitrend</t>
+  </si>
+  <si>
+    <t>verapam</t>
+  </si>
+  <si>
+    <t>diltiaz</t>
+  </si>
+  <si>
+    <t>doxazos</t>
+  </si>
+  <si>
+    <t>minoxid</t>
+  </si>
+  <si>
+    <t>dialisis</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1577,6 +2003,13 @@
       <color rgb="FF3BA7C7"/>
       <name val="DinBold"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1599,10 +2032,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1924,1818 +2362,1819 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3478553-F71F-AA43-AE48-761FD61CF1E4}">
   <dimension ref="A1:D129"/>
   <sheetViews>
-    <sheetView topLeftCell="A118" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="C138" sqref="C138"/>
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="76.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="76.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="10.6640625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="5" t="s">
         <v>234</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="5" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="C2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="C3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="C4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="C5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="C6" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="C7" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="C8" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="C9" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="C10" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="C11" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="C12" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C13" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="C13" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C14" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" t="s">
+      <c r="C14" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C15" t="s">
-        <v>4</v>
-      </c>
-      <c r="D15" t="s">
+      <c r="C15" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C16" t="s">
-        <v>4</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="C16" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C17" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="C17" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C18" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" t="s">
+      <c r="C18" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C19" t="s">
-        <v>4</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="C19" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C20" t="s">
-        <v>4</v>
-      </c>
-      <c r="D20" t="s">
+      <c r="C20" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C21" t="s">
-        <v>4</v>
-      </c>
-      <c r="D21" t="s">
+      <c r="C21" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C22" t="s">
-        <v>4</v>
-      </c>
-      <c r="D22" t="s">
+      <c r="C22" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C23" t="s">
-        <v>4</v>
-      </c>
-      <c r="D23" t="s">
+      <c r="C23" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C24" t="s">
-        <v>4</v>
-      </c>
-      <c r="D24" t="s">
+      <c r="C24" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C25" t="s">
-        <v>4</v>
-      </c>
-      <c r="D25" t="s">
+      <c r="C25" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C26" t="s">
-        <v>4</v>
-      </c>
-      <c r="D26" t="s">
+      <c r="C26" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C27" t="s">
-        <v>4</v>
-      </c>
-      <c r="D27" t="s">
+      <c r="C27" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C28" t="s">
-        <v>4</v>
-      </c>
-      <c r="D28" t="s">
+      <c r="C28" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D28" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C29" t="s">
-        <v>4</v>
-      </c>
-      <c r="D29" t="s">
+      <c r="C29" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C30" t="s">
-        <v>4</v>
-      </c>
-      <c r="D30" t="s">
+      <c r="C30" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C31" t="s">
-        <v>4</v>
-      </c>
-      <c r="D31" t="s">
+      <c r="C31" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D31" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C32" t="s">
-        <v>4</v>
-      </c>
-      <c r="D32" t="s">
+      <c r="C32" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D32" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="C33" t="s">
-        <v>4</v>
-      </c>
-      <c r="D33" t="s">
+      <c r="C33" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D33" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C34" t="s">
-        <v>4</v>
-      </c>
-      <c r="D34" t="s">
+      <c r="C34" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D34" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C35" t="s">
-        <v>4</v>
-      </c>
-      <c r="D35" t="s">
+      <c r="C35" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D35" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="C36" t="s">
-        <v>4</v>
-      </c>
-      <c r="D36" t="s">
+      <c r="C36" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D36" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="C37" t="s">
-        <v>4</v>
-      </c>
-      <c r="D37" t="s">
+      <c r="C37" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D37" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="C38" t="s">
-        <v>4</v>
-      </c>
-      <c r="D38" t="s">
+      <c r="C38" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D38" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="C39" t="s">
-        <v>4</v>
-      </c>
-      <c r="D39" t="s">
+      <c r="C39" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D39" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="C40" t="s">
-        <v>4</v>
-      </c>
-      <c r="D40" t="s">
+      <c r="C40" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D40" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="C41" t="s">
-        <v>4</v>
-      </c>
-      <c r="D41" t="s">
+      <c r="C41" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D41" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="C42" t="s">
-        <v>4</v>
-      </c>
-      <c r="D42" t="s">
+      <c r="C42" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D42" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="C43" t="s">
-        <v>4</v>
-      </c>
-      <c r="D43" t="s">
+      <c r="C43" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D43" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="C44" t="s">
-        <v>4</v>
-      </c>
-      <c r="D44" t="s">
+      <c r="C44" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D44" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="C45" t="s">
-        <v>4</v>
-      </c>
-      <c r="D45" t="s">
+      <c r="C45" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D45" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="C46" t="s">
-        <v>4</v>
-      </c>
-      <c r="D46" t="s">
+      <c r="C46" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D46" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="C47" t="s">
-        <v>4</v>
-      </c>
-      <c r="D47" t="s">
+      <c r="C47" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D47" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="C48" t="s">
-        <v>4</v>
-      </c>
-      <c r="D48" t="s">
+      <c r="C48" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D48" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="C49" t="s">
-        <v>4</v>
-      </c>
-      <c r="D49" t="s">
+      <c r="C49" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D49" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A50" t="s">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="C50" t="s">
-        <v>4</v>
-      </c>
-      <c r="D50" t="s">
+      <c r="C50" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D50" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A51" t="s">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="C51" t="s">
-        <v>4</v>
-      </c>
-      <c r="D51" t="s">
+      <c r="C51" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D51" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A52" t="s">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="C52" t="s">
-        <v>4</v>
-      </c>
-      <c r="D52" t="s">
+      <c r="C52" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D52" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A53" t="s">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="C53" t="s">
-        <v>4</v>
-      </c>
-      <c r="D53" t="s">
+      <c r="C53" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D53" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A54" t="s">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B54" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="C54" t="s">
-        <v>4</v>
-      </c>
-      <c r="D54" t="s">
+      <c r="C54" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D54" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A55" t="s">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="C55" t="s">
-        <v>4</v>
-      </c>
-      <c r="D55" t="s">
+      <c r="C55" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D55" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A56" t="s">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="C56" t="s">
-        <v>4</v>
-      </c>
-      <c r="D56" t="s">
+      <c r="C56" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D56" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A57" t="s">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="C57" t="s">
-        <v>4</v>
-      </c>
-      <c r="D57" t="s">
+      <c r="C57" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D57" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A58" t="s">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B58" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="C58" t="s">
-        <v>4</v>
-      </c>
-      <c r="D58" t="s">
+      <c r="C58" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D58" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A59" t="s">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B59" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="C59" t="s">
-        <v>4</v>
-      </c>
-      <c r="D59" t="s">
+      <c r="C59" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D59" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A60" t="s">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B60" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="C60" t="s">
-        <v>4</v>
-      </c>
-      <c r="D60" t="s">
+      <c r="C60" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D60" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A61" t="s">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B61" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="C61" t="s">
-        <v>4</v>
-      </c>
-      <c r="D61" t="s">
+      <c r="C61" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D61" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A62" t="s">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B62" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="C62" t="s">
-        <v>4</v>
-      </c>
-      <c r="D62" t="s">
+      <c r="C62" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D62" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A63" t="s">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63" s="5" t="s">
         <v>237</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B63" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="C63" t="s">
-        <v>236</v>
-      </c>
-      <c r="D63" t="s">
+      <c r="C63" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="D63" s="5" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A64" t="s">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B64" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="C64" t="s">
-        <v>236</v>
-      </c>
-      <c r="D64" t="s">
+      <c r="C64" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="D64" s="5" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A65" t="s">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B65" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="C65" t="s">
-        <v>236</v>
-      </c>
-      <c r="D65" t="s">
+      <c r="C65" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="D65" s="5" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A66" t="s">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B66" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="C66" t="s">
-        <v>236</v>
-      </c>
-      <c r="D66" t="s">
+      <c r="C66" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="D66" s="5" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A67" t="s">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B67" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="C67" t="s">
-        <v>236</v>
-      </c>
-      <c r="D67" t="s">
+      <c r="C67" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="D67" s="5" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A68" t="s">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B68" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="C68" t="s">
-        <v>236</v>
-      </c>
-      <c r="D68" t="s">
+      <c r="C68" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="D68" s="5" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A69" t="s">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B69" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="C69" t="s">
-        <v>236</v>
-      </c>
-      <c r="D69" t="s">
+      <c r="C69" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="D69" s="5" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A70" t="s">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B70" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="C70" t="s">
-        <v>236</v>
-      </c>
-      <c r="D70" t="s">
+      <c r="C70" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="D70" s="5" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A71" t="s">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B71" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="C71" t="s">
-        <v>236</v>
-      </c>
-      <c r="D71" t="s">
+      <c r="C71" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="D71" s="5" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A72" t="s">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B72" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="C72" t="s">
-        <v>236</v>
-      </c>
-      <c r="D72" t="s">
+      <c r="C72" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="D72" s="5" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A73" t="s">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A73" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B73" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="C73" t="s">
-        <v>236</v>
-      </c>
-      <c r="D73" t="s">
+      <c r="C73" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="D73" s="5" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A74" t="s">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B74" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="C74" t="s">
-        <v>236</v>
-      </c>
-      <c r="D74" t="s">
+      <c r="C74" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="D74" s="5" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A75" t="s">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B75" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="C75" t="s">
-        <v>236</v>
-      </c>
-      <c r="D75" t="s">
+      <c r="C75" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="D75" s="5" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A76" t="s">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A76" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B76" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="C76" t="s">
-        <v>236</v>
-      </c>
-      <c r="D76" t="s">
+      <c r="C76" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="D76" s="5" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A77" t="s">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A77" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B77" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="C77" t="s">
-        <v>236</v>
-      </c>
-      <c r="D77" t="s">
+      <c r="C77" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="D77" s="5" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A78" t="s">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A78" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B78" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="C78" t="s">
-        <v>236</v>
-      </c>
-      <c r="D78" t="s">
+      <c r="C78" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="D78" s="5" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A79" t="s">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A79" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B79" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="C79" t="s">
-        <v>236</v>
-      </c>
-      <c r="D79" t="s">
+      <c r="C79" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="D79" s="5" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A80" t="s">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A80" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B80" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="C80" t="s">
-        <v>236</v>
-      </c>
-      <c r="D80" t="s">
+      <c r="C80" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="D80" s="5" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A81" t="s">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A81" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B81" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="C81" t="s">
-        <v>236</v>
-      </c>
-      <c r="D81" t="s">
+      <c r="C81" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="D81" s="5" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A82" t="s">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A82" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B82" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="C82" t="s">
-        <v>236</v>
-      </c>
-      <c r="D82" t="s">
+      <c r="C82" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="D82" s="5" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A83" t="s">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A83" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B83" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="C83" t="s">
-        <v>236</v>
-      </c>
-      <c r="D83" t="s">
+      <c r="C83" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="D83" s="5" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A84" t="s">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A84" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B84" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="C84" t="s">
-        <v>236</v>
-      </c>
-      <c r="D84" t="s">
+      <c r="C84" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="D84" s="5" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A85" t="s">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A85" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B85" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="C85" t="s">
-        <v>236</v>
-      </c>
-      <c r="D85" t="s">
+      <c r="C85" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="D85" s="5" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A86" t="s">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A86" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B86" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="C86" t="s">
-        <v>236</v>
-      </c>
-      <c r="D86" t="s">
+      <c r="C86" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="D86" s="5" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A87" t="s">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A87" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B87" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="C87" t="s">
-        <v>236</v>
-      </c>
-      <c r="D87" t="s">
+      <c r="C87" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="D87" s="5" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A88" t="s">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A88" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B88" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="C88" t="s">
-        <v>236</v>
-      </c>
-      <c r="D88" t="s">
+      <c r="C88" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="D88" s="5" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A89" t="s">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A89" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="B89" t="s">
+      <c r="B89" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="C89" t="s">
-        <v>236</v>
-      </c>
-      <c r="D89" t="s">
+      <c r="C89" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="D89" s="5" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A90" t="s">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A90" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B90" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="C90" t="s">
-        <v>236</v>
-      </c>
-      <c r="D90" t="s">
+      <c r="C90" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="D90" s="5" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A91" t="s">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A91" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="B91" t="s">
+      <c r="B91" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="C91" t="s">
-        <v>236</v>
-      </c>
-      <c r="D91" t="s">
+      <c r="C91" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="D91" s="5" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A92" t="s">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A92" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="B92" t="s">
+      <c r="B92" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="C92" t="s">
-        <v>236</v>
-      </c>
-      <c r="D92" t="s">
+      <c r="C92" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="D92" s="5" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A93" t="s">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A93" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B93" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="C93" t="s">
-        <v>236</v>
-      </c>
-      <c r="D93" t="s">
+      <c r="C93" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="D93" s="5" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A94" t="s">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A94" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B94" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="C94" t="s">
-        <v>236</v>
-      </c>
-      <c r="D94" t="s">
+      <c r="C94" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="D94" s="5" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A95" t="s">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A95" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="B95" t="s">
+      <c r="B95" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="C95" t="s">
-        <v>236</v>
-      </c>
-      <c r="D95" t="s">
+      <c r="C95" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="D95" s="5" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A96" t="s">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A96" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B96" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="C96" t="s">
-        <v>236</v>
-      </c>
-      <c r="D96" t="s">
+      <c r="C96" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="D96" s="5" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A97" t="s">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A97" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="B97" t="s">
+      <c r="B97" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="C97" t="s">
-        <v>236</v>
-      </c>
-      <c r="D97" t="s">
+      <c r="C97" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="D97" s="5" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A98" t="s">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A98" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B98" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="C98" t="s">
-        <v>236</v>
-      </c>
-      <c r="D98" t="s">
+      <c r="C98" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="D98" s="5" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A99" t="s">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A99" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="B99" t="s">
+      <c r="B99" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="C99" t="s">
-        <v>236</v>
-      </c>
-      <c r="D99" t="s">
+      <c r="C99" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="D99" s="5" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A100" t="s">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A100" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="B100" t="s">
+      <c r="B100" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="C100" t="s">
-        <v>236</v>
-      </c>
-      <c r="D100" t="s">
+      <c r="C100" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="D100" s="5" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A101" t="s">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A101" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="B101" t="s">
+      <c r="B101" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="C101" t="s">
-        <v>236</v>
-      </c>
-      <c r="D101" t="s">
+      <c r="C101" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="D101" s="5" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A102" t="s">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A102" s="5" t="s">
         <v>191</v>
       </c>
-      <c r="B102" t="s">
+      <c r="B102" s="5" t="s">
         <v>192</v>
       </c>
-      <c r="C102" t="s">
-        <v>236</v>
-      </c>
-      <c r="D102" t="s">
+      <c r="C102" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="D102" s="5" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A103" t="s">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A103" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="B103" t="s">
+      <c r="B103" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="C103" t="s">
-        <v>236</v>
-      </c>
-      <c r="D103" t="s">
+      <c r="C103" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="D103" s="5" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A104" t="s">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A104" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="B104" t="s">
+      <c r="B104" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="C104" t="s">
-        <v>236</v>
-      </c>
-      <c r="D104" t="s">
+      <c r="C104" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="D104" s="5" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A105" t="s">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A105" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="B105" t="s">
+      <c r="B105" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="C105" t="s">
-        <v>236</v>
-      </c>
-      <c r="D105" t="s">
+      <c r="C105" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="D105" s="5" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A106" t="s">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A106" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="B106" t="s">
+      <c r="B106" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="C106" t="s">
-        <v>236</v>
-      </c>
-      <c r="D106" t="s">
+      <c r="C106" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="D106" s="5" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A107" t="s">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A107" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="B107" t="s">
+      <c r="B107" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="C107" t="s">
-        <v>236</v>
-      </c>
-      <c r="D107" t="s">
+      <c r="C107" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="D107" s="5" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A108" t="s">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A108" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="B108" t="s">
+      <c r="B108" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="C108" t="s">
-        <v>236</v>
-      </c>
-      <c r="D108" t="s">
+      <c r="C108" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="D108" s="5" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A109" t="s">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A109" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="B109" t="s">
+      <c r="B109" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="C109" t="s">
-        <v>236</v>
-      </c>
-      <c r="D109" t="s">
+      <c r="C109" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="D109" s="5" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A110" t="s">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A110" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="B110" t="s">
+      <c r="B110" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="C110" t="s">
-        <v>236</v>
-      </c>
-      <c r="D110" t="s">
+      <c r="C110" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="D110" s="5" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A111" t="s">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A111" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="B111" t="s">
+      <c r="B111" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="C111" t="s">
-        <v>236</v>
-      </c>
-      <c r="D111" t="s">
+      <c r="C111" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="D111" s="5" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A112" t="s">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A112" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="B112" t="s">
+      <c r="B112" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="C112" t="s">
-        <v>236</v>
-      </c>
-      <c r="D112" t="s">
+      <c r="C112" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="D112" s="5" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A113" t="s">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A113" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="B113" t="s">
+      <c r="B113" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="C113" t="s">
-        <v>236</v>
-      </c>
-      <c r="D113" t="s">
+      <c r="C113" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="D113" s="5" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A114" t="s">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A114" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="B114" t="s">
+      <c r="B114" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="C114" t="s">
-        <v>236</v>
-      </c>
-      <c r="D114" t="s">
+      <c r="C114" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="D114" s="5" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A115" t="s">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A115" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="B115" t="s">
+      <c r="B115" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="C115" t="s">
-        <v>236</v>
-      </c>
-      <c r="D115" t="s">
+      <c r="C115" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="D115" s="5" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A116" t="s">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A116" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="B116" t="s">
+      <c r="B116" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="C116" t="s">
-        <v>236</v>
-      </c>
-      <c r="D116" t="s">
+      <c r="C116" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="D116" s="5" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A117" t="s">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A117" s="5" t="s">
         <v>221</v>
       </c>
-      <c r="B117" t="s">
+      <c r="B117" s="5" t="s">
         <v>222</v>
       </c>
-      <c r="C117" t="s">
-        <v>236</v>
-      </c>
-      <c r="D117" t="s">
+      <c r="C117" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="D117" s="5" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A118" t="s">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A118" s="5" t="s">
         <v>223</v>
       </c>
-      <c r="B118" t="s">
+      <c r="B118" s="5" t="s">
         <v>224</v>
       </c>
-      <c r="C118" t="s">
-        <v>236</v>
-      </c>
-      <c r="D118" t="s">
+      <c r="C118" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="D118" s="5" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A119" t="s">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A119" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="B119" t="s">
+      <c r="B119" s="5" t="s">
         <v>226</v>
       </c>
-      <c r="C119" t="s">
-        <v>236</v>
-      </c>
-      <c r="D119" t="s">
+      <c r="C119" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="D119" s="5" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A120" t="s">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A120" s="5" t="s">
         <v>227</v>
       </c>
-      <c r="B120" t="s">
+      <c r="B120" s="5" t="s">
         <v>228</v>
       </c>
-      <c r="C120" t="s">
-        <v>236</v>
-      </c>
-      <c r="D120" t="s">
+      <c r="C120" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="D120" s="5" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A121" t="s">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A121" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="B121" t="s">
+      <c r="B121" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="C121" t="s">
-        <v>236</v>
-      </c>
-      <c r="D121" t="s">
+      <c r="C121" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="D121" s="5" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A122" t="s">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A122" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="B122" t="s">
+      <c r="B122" s="5" t="s">
         <v>231</v>
       </c>
-      <c r="C122" t="s">
-        <v>236</v>
-      </c>
-      <c r="D122" t="s">
+      <c r="C122" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="D122" s="5" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A123" t="s">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A123" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="B123" t="s">
+      <c r="B123" s="5" t="s">
         <v>232</v>
       </c>
-      <c r="C123" t="s">
-        <v>236</v>
-      </c>
-      <c r="D123" t="s">
+      <c r="C123" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="D123" s="5" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A124" t="s">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A124" s="5" t="s">
         <v>238</v>
       </c>
-      <c r="B124">
+      <c r="B124" s="5">
         <v>893911</v>
       </c>
-      <c r="C124" t="s">
+      <c r="C124" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="D124" t="s">
+      <c r="D124" s="5" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A125" t="s">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A125" s="5" t="s">
         <v>233</v>
       </c>
-      <c r="B125">
+      <c r="B125" s="5">
         <v>903883</v>
       </c>
-      <c r="C125" t="s">
+      <c r="C125" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="D125" t="s">
+      <c r="D125" s="5" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A126" t="s">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A126" s="5" t="s">
         <v>239</v>
       </c>
-      <c r="B126">
+      <c r="B126" s="5">
         <v>904702</v>
       </c>
-      <c r="C126" t="s">
+      <c r="C126" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="D126" t="s">
+      <c r="D126" s="5" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A127" t="s">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A127" s="5" t="s">
         <v>240</v>
       </c>
-      <c r="B127">
+      <c r="B127" s="5">
         <v>904703</v>
       </c>
-      <c r="C127" t="s">
+      <c r="C127" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="D127" t="s">
+      <c r="D127" s="5" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A128" t="s">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A128" s="5" t="s">
         <v>241</v>
       </c>
-      <c r="B128">
+      <c r="B128" s="5">
         <v>903426</v>
       </c>
-      <c r="C128" t="s">
+      <c r="C128" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="D128" t="s">
+      <c r="D128" s="5" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A129" t="s">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A129" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="B129">
+      <c r="B129" s="5">
         <v>903427</v>
       </c>
-      <c r="C129" t="s">
+      <c r="C129" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="D129" t="s">
+      <c r="D129" s="5" t="s">
         <v>269</v>
       </c>
     </row>
@@ -3745,11 +4184,1376 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7B4A71D-3876-46CB-BEA5-ECF7A1BE0A88}">
+  <dimension ref="A1:D95"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="16384" width="10.6640625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>504</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>508</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>510</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>516</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>519</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>529</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>531</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>532</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>535</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>540</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>541</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>546</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>548</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>549</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>550</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>551</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>552</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>553</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>555</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>558</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>559</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>560</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>561</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>562</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>563</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>564</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>565</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>566</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>568</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>570</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>571</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" s="3" t="s">
+        <v>533</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" s="3" t="s">
+        <v>537</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" s="3" t="s">
+        <v>542</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" s="3" t="s">
+        <v>368</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66" s="3" t="s">
+        <v>422</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" s="3" t="s">
+        <v>569</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" s="3" t="s">
+        <v>572</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69" s="3" t="s">
+        <v>573</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70" s="3" t="s">
+        <v>574</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>575</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" s="3" t="s">
+        <v>576</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72" s="3" t="s">
+        <v>577</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A73" s="3" t="s">
+        <v>578</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A76" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A77" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A78" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A79" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A80" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A81" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A82" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="B82" s="1">
+        <v>389500</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A83" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="B83" s="1">
+        <v>392701</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A84" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="B84" s="1">
+        <v>392702</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A85" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="B85" s="1">
+        <v>394200</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A86" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="B86" s="1">
+        <v>394300</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A87" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="B87" s="1">
+        <v>399501</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A88" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="B88" s="1">
+        <v>549001</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A89" s="1" t="s">
+        <v>521</v>
+      </c>
+      <c r="B89" s="1">
+        <v>549002</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A90" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B90" s="1">
+        <v>549012</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A91" s="1" t="s">
+        <v>527</v>
+      </c>
+      <c r="B91" s="1">
+        <v>549800</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A92" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="B92" s="1">
+        <v>549801</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A93" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="B93" s="1">
+        <v>549802</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A94" s="1" t="s">
+        <v>538</v>
+      </c>
+      <c r="B94" s="4" t="s">
+        <v>539</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A95" s="1" t="s">
+        <v>543</v>
+      </c>
+      <c r="B95" s="4" t="s">
+        <v>544</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>635</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="A54" r:id="rId1" tooltip="Eprosartán (aún no redactado)" display="https://es.wikipedia.org/w/index.php?title=Eprosart%C3%A1n&amp;action=edit&amp;redlink=1" xr:uid="{8CA33493-8BF9-436E-9445-477A640CE7D7}"/>
+    <hyperlink ref="A55" r:id="rId2" tooltip="Valsartán" display="https://es.wikipedia.org/wiki/Valsart%C3%A1n" xr:uid="{362C5B92-BEA8-44ED-ABCD-E31F9CFC37DA}"/>
+    <hyperlink ref="A56" r:id="rId3" tooltip="Irbesartán" display="https://es.wikipedia.org/wiki/Irbesart%C3%A1n" xr:uid="{71225374-638F-4E66-AB73-BBC25402B324}"/>
+    <hyperlink ref="A57" r:id="rId4" tooltip="Candesartán" display="https://es.wikipedia.org/wiki/Candesart%C3%A1n" xr:uid="{F4DCEA31-05AC-4288-863A-7053F33A9222}"/>
+    <hyperlink ref="A58" r:id="rId5" tooltip="Telmisartán" display="https://es.wikipedia.org/wiki/Telmisart%C3%A1n" xr:uid="{E9080C87-77C8-4B9B-8E74-54B7E7E3C2DF}"/>
+    <hyperlink ref="A59" r:id="rId6" tooltip="Olmesartán" display="https://es.wikipedia.org/wiki/Olmesart%C3%A1n" xr:uid="{8FBBD847-5633-419F-9238-231F8E90FBB5}"/>
+    <hyperlink ref="A66" r:id="rId7" tooltip="Amlodipino" display="https://es.wikipedia.org/wiki/Amlodipino" xr:uid="{54164E03-24D1-4177-A857-91520FCE5791}"/>
+    <hyperlink ref="A67" r:id="rId8" tooltip="Felodipino" display="https://es.wikipedia.org/wiki/Felodipino" xr:uid="{C9E59EEB-E0AD-4153-9637-F110818DA40B}"/>
+    <hyperlink ref="A68" r:id="rId9" tooltip="Isradipino (aún no redactado)" display="https://es.wikipedia.org/w/index.php?title=Isradipino&amp;action=edit&amp;redlink=1" xr:uid="{9DA77BA0-0EAF-481E-A842-4354D4A05F6F}"/>
+    <hyperlink ref="A69" r:id="rId10" tooltip="Nicardipino" display="https://es.wikipedia.org/wiki/Nicardipino" xr:uid="{E0A6E207-F0CC-40A7-9162-BE309D5234A7}"/>
+    <hyperlink ref="A70" r:id="rId11" tooltip="Nifedipino" display="https://es.wikipedia.org/wiki/Nifedipino" xr:uid="{05A1B899-E4E9-4FB8-9A53-D6520725F368}"/>
+    <hyperlink ref="A71" r:id="rId12" tooltip="Nimodipino" display="https://es.wikipedia.org/wiki/Nimodipino" xr:uid="{E842FC86-04E5-44CB-8EFF-09BDE28C3C7A}"/>
+    <hyperlink ref="A72" r:id="rId13" tooltip="Nisoldipino" display="https://es.wikipedia.org/wiki/Nisoldipino" xr:uid="{461E3521-4711-4079-A157-F1474238008A}"/>
+    <hyperlink ref="A73" r:id="rId14" tooltip="Nitrendipino" display="https://es.wikipedia.org/wiki/Nitrendipino" xr:uid="{89AD1012-7676-4B81-8670-C567F702E796}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F7A4EE8-9C1A-4345-81FE-4CE18C64706F}">
   <dimension ref="A1:D98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -5157,18 +6961,4 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AF2E5EF-8401-1241-A402-0FF58C96F248}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>